<commit_message>
`app.js` working version of import of `loadrealized`, just need to sync `async` functions
</commit_message>
<xml_diff>
--- a/app/utils/excel-parser-scripts/auctions/auctions-auto.xlsx
+++ b/app/utils/excel-parser-scripts/auctions/auctions-auto.xlsx
@@ -1271,13 +1271,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1294,8 +1293,85 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1304,12 +1380,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1317,8 +1435,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1342,25 +1475,153 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1372,7 +1633,7 @@
   <dimension ref="A1:BY337"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G354" activeCellId="0" sqref="G354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1382,9 +1643,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="6" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="11" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="30" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="16.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="78" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>